<commit_message>
kleine tekstuele aanpassingen bij toelichting
</commit_message>
<xml_diff>
--- a/Beheren standaarden KLIC/Eisen overheid ordening attributen (concept).xlsx
+++ b/Beheren standaarden KLIC/Eisen overheid ordening attributen (concept).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hetkadaster.sharepoint.com/sites/KLIC/Shared Documents/Documentatie Functioneel/KLIC-WIN/9900 Requirements/80. Standaarden, IMKL/_prioritering (attributen)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="286" documentId="8_{71E0E571-F757-4273-913E-5437407046B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{CB9653B7-A70C-4738-9E15-521EC3A51A7E}"/>
+  <xr:revisionPtr revIDLastSave="293" documentId="8_{71E0E571-F757-4273-913E-5437407046B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{20E9BABD-85F6-48C8-8160-8238ACE77D8D}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{149DC1E7-FAE5-417C-8DC6-87A35A16D8AD}"/>
   </bookViews>
@@ -3041,7 +3041,19 @@
         <a:p>
           <a:r>
             <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
-            <a:t>Daartoe heeft de Technische Commissie Standaarden KLIC (TCS) een voorstel uitgewerkt.</a:t>
+            <a:t>Daartoe heeft de Technische Commissie Standaarden KLIC (TCS) </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>dit</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
+            <a:t> voorstel uitgewerkt.</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -3226,8 +3238,28 @@
         <a:p>
           <a:r>
             <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
-            <a:t>  &gt; de waarschijnlijkheid dat een attribuutwaarde gevuld wordt (verplicht, optioneel); zie daarvoor de legenda tabblad 'Ordening'</a:t>
+            <a:t>  &gt; de waarschijnlijkheid dat een attribuutwaarde gevuld wordt (verplicht, optioneel); zie daarvoor de legenda op de tabbladen</a:t>
           </a:r>
+          <a:br>
+            <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
+          </a:br>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
+            <a:t>     'Ordening (TCS)' en </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>'Ordening (TCS) (NL)'</a:t>
+          </a:r>
+          <a:endParaRPr lang="nl-NL" sz="1100" baseline="0"/>
         </a:p>
         <a:p>
           <a:r>
@@ -4491,7 +4523,7 @@
   <dimension ref="A1:AP139"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="2" topLeftCell="G108" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="G3" sqref="G3"/>
@@ -29515,21 +29547,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010072E6CDABC94C8E4D9FF787BE52A12D70" ma:contentTypeVersion="10" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="42d04a1539dbe8e7765031e6c6055247">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b4710195-8c97-40d8-961f-382a10a2b3ee" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c33fada9a9359e767f1806f1464d746a" ns2:_="">
     <xsd:import namespace="b4710195-8c97-40d8-961f-382a10a2b3ee"/>
@@ -29713,7 +29730,26 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{59BFED2B-F51F-47DD-BB82-3A6F146ED94F}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E666C7DC-BABB-45EF-8C3F-0881662747CC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -29729,14 +29765,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C1902ECF-A93E-435D-908F-0926C6EE1B5F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B93EE77A-7569-47CE-B6D9-2C2C461E906F}"/>
 </file>
</xml_diff>